<commit_message>
moving towards final version, issues tackled are listed in issues
</commit_message>
<xml_diff>
--- a/data/Course Booklet 2019/AI_PG_Curriculum.xlsx
+++ b/data/Course Booklet 2019/AI_PG_Curriculum.xlsx
@@ -45,13 +45,13 @@
     <t>EE5827</t>
   </si>
   <si>
-    <t>CS6013</t>
-  </si>
-  <si>
     <t>EE5609</t>
   </si>
   <si>
     <t>EE5600</t>
+  </si>
+  <si>
+    <t>CS6013</t>
   </si>
   <si>
     <t>EE5601</t>
@@ -63,16 +63,16 @@
     <t>EE5603</t>
   </si>
   <si>
+    <t>EE5604</t>
+  </si>
+  <si>
+    <t>EE5605</t>
+  </si>
+  <si>
     <t>EE/CS/MA</t>
   </si>
   <si>
     <t>Core Electives</t>
-  </si>
-  <si>
-    <t>EE5604</t>
-  </si>
-  <si>
-    <t>EE5605</t>
   </si>
   <si>
     <t>EE5606</t>
@@ -93,28 +93,28 @@
     <t>EE5608</t>
   </si>
   <si>
-    <t>Summer</t>
+    <t>EE5925</t>
   </si>
   <si>
-    <t>EE5925</t>
+    <t>Summer</t>
   </si>
   <si>
     <t>FE</t>
   </si>
   <si>
-    <t>EE5935</t>
-  </si>
-  <si>
     <t>Free Electives</t>
-  </si>
-  <si>
-    <t>EE5945</t>
   </si>
   <si>
     <t>EE5815</t>
   </si>
   <si>
+    <t>EE5935</t>
+  </si>
+  <si>
     <t>EE5825</t>
+  </si>
+  <si>
+    <t>EE5945</t>
   </si>
   <si>
     <t>EE5835</t>
@@ -314,7 +314,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
@@ -346,7 +346,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
@@ -378,7 +378,7 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
@@ -474,10 +474,10 @@
         <v>1.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3">
         <v>3.0</v>
@@ -542,7 +542,7 @@
         <v>2.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
@@ -574,7 +574,7 @@
         <v>2.0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
@@ -766,10 +766,10 @@
         <v>2.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D18" s="3">
         <v>6.0</v>
@@ -799,13 +799,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D19" s="3">
         <v>3.0</v>
@@ -835,13 +835,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="2"/>
@@ -7385,7 +7385,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
@@ -7417,7 +7417,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
@@ -7449,7 +7449,7 @@
         <v>1.0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
@@ -7577,7 +7577,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
@@ -7609,7 +7609,7 @@
         <v>2.0</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
@@ -7801,10 +7801,10 @@
         <v>2.0</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D17" s="3">
         <v>3.0</v>
@@ -7837,7 +7837,7 @@
         <v>2.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="3"/>
@@ -7866,10 +7866,10 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
@@ -14481,7 +14481,7 @@
         <v>1.0</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
@@ -14513,7 +14513,7 @@
         <v>1.0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
@@ -14641,7 +14641,7 @@
         <v>2.0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="3"/>
@@ -14673,7 +14673,7 @@
         <v>2.0</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
@@ -14801,7 +14801,7 @@
         <v>3.0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3"/>
@@ -14833,10 +14833,10 @@
         <v>3.0</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D15" s="3">
         <v>3.0</v>
@@ -14965,7 +14965,7 @@
         <v>4.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="3"/>
@@ -14997,7 +14997,7 @@
         <v>5.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3"/>
@@ -15029,7 +15029,7 @@
         <v>6.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>

</xml_diff>